<commit_message>
+fonction d'affichage des tableau +fonction d'affichage de la matrice de connections +fonction d'entree de prediction
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="17540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="moy10" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9856" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9858" uniqueCount="19">
   <si>
     <t xml:space="preserve">passe nÂ° </t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>ERREUR</t>
+  </si>
+  <si>
+    <t>topologie</t>
+  </si>
+  <si>
+    <t>2 4 1</t>
   </si>
 </sst>
 </file>
@@ -8793,7 +8799,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="140" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -85157,10 +85163,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -85218,6 +85224,14 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout de .gitignore et divers modif
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="17540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="17540" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="moy10" sheetId="2" r:id="rId1"/>
     <sheet name="ErreurInstantanée" sheetId="3" r:id="rId2"/>
     <sheet name="Feuil1" sheetId="1" r:id="rId3"/>
     <sheet name="Feuil2" sheetId="4" r:id="rId4"/>
+    <sheet name="Feuil3" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Feuil1!$A$1:$B$8442</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9858" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9908" uniqueCount="30">
   <si>
     <t xml:space="preserve">passe nÂ° </t>
   </si>
@@ -90,11 +91,47 @@
   <si>
     <t>2 4 1</t>
   </si>
+  <si>
+    <t>Neurone</t>
+  </si>
+  <si>
+    <t>[0][0]</t>
+  </si>
+  <si>
+    <t>-&gt;</t>
+  </si>
+  <si>
+    <t>[1][0]</t>
+  </si>
+  <si>
+    <t>[1][1]</t>
+  </si>
+  <si>
+    <t>[1][2]</t>
+  </si>
+  <si>
+    <t>[1][3]</t>
+  </si>
+  <si>
+    <t>[0][1]</t>
+  </si>
+  <si>
+    <t>[0][2]</t>
+  </si>
+  <si>
+    <t>[2][0]</t>
+  </si>
+  <si>
+    <t>[1][4]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -124,9 +161,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4414,11 +4453,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2100436464"/>
-        <c:axId val="-2100617680"/>
+        <c:axId val="2091515456"/>
+        <c:axId val="2137150448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2100436464"/>
+        <c:axId val="2091515456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4427,7 +4466,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2100617680"/>
+        <c:crossAx val="2137150448"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4435,7 +4474,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2100617680"/>
+        <c:axId val="2137150448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -4447,7 +4486,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2100436464"/>
+        <c:crossAx val="2091515456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4489,7 +4528,6 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:trendline>
-            <c:name/>
             <c:trendlineType val="movingAvg"/>
             <c:period val="150"/>
             <c:dispRSqr val="0"/>
@@ -8739,11 +8777,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1769537664"/>
-        <c:axId val="-2005768432"/>
+        <c:axId val="2139262272"/>
+        <c:axId val="2142072960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1769537664"/>
+        <c:axId val="2139262272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8752,7 +8790,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2005768432"/>
+        <c:crossAx val="2142072960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8760,7 +8798,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2005768432"/>
+        <c:axId val="2142072960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -8772,7 +8810,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1769537664"/>
+        <c:crossAx val="2139262272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8810,7 +8848,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9289143" cy="6059714"/>
+    <xdr:ext cx="9298214" cy="6059714"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1"/>
@@ -8837,7 +8875,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9289143" cy="6059714"/>
+    <xdr:ext cx="9298214" cy="6059714"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1"/>
@@ -8857,6 +8895,1381 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>6096</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Ellipse 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4127500" y="1016000"/>
+          <a:ext cx="1225296" cy="1225296"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>6096</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Ellipse 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4127500" y="3860800"/>
+          <a:ext cx="1225296" cy="1225296"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>108204</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Ellipse 7"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3302000" y="6610604"/>
+          <a:ext cx="1225296" cy="1225296"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="3200">
+              <a:latin typeface="Courier New" charset="0"/>
+              <a:ea typeface="Courier New" charset="0"/>
+              <a:cs typeface="Courier New" charset="0"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>6096</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Ellipse 8"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8109204" y="203200"/>
+          <a:ext cx="1225296" cy="1225296"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>197104</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Ellipse 9"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8109204" y="1619504"/>
+          <a:ext cx="1225296" cy="1225296"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>6096</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Ellipse 10"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8109204" y="3048000"/>
+          <a:ext cx="1225296" cy="1225296"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>6096</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Ellipse 11"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8109204" y="4470400"/>
+          <a:ext cx="1225296" cy="1225296"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>197104</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Ellipse 13"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7283704" y="5886704"/>
+          <a:ext cx="1225296" cy="1225296"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="3200">
+              <a:latin typeface="Courier New" charset="0"/>
+              <a:ea typeface="Courier New" charset="0"/>
+              <a:cs typeface="Courier New" charset="0"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>197104</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Ellipse 14"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11557000" y="3854704"/>
+          <a:ext cx="1225296" cy="1225296"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Connecteur droit avec flèche 16"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5352796" y="812800"/>
+          <a:ext cx="2756408" cy="815848"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="58419">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>200152</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Connecteur droit avec flèche 17"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="6"/>
+          <a:endCxn id="10" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5352796" y="1628648"/>
+          <a:ext cx="2756408" cy="603504"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="20320">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Connecteur droit avec flèche 20"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="6"/>
+          <a:endCxn id="11" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5352796" y="1628648"/>
+          <a:ext cx="2756408" cy="2032000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="27940">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>155956</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Connecteur droit avec flèche 23"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5352796" y="1628648"/>
+          <a:ext cx="2756408" cy="3404108"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="100330">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Connecteur droit avec flèche 30"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="6"/>
+          <a:endCxn id="9" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5352796" y="815848"/>
+          <a:ext cx="2756408" cy="3657600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="54610">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>200152</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Connecteur droit avec flèche 33"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="6"/>
+          <a:endCxn id="10" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5352796" y="2232152"/>
+          <a:ext cx="2756408" cy="2241296"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="20320">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Connecteur droit avec flèche 36"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5352796" y="3657600"/>
+          <a:ext cx="2756408" cy="815848"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="17780">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>155956</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Connecteur droit avec flèche 39"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5352796" y="4473448"/>
+          <a:ext cx="2756408" cy="559308"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="77470">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Connecteur droit avec flèche 45"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="9" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5352796" y="815848"/>
+          <a:ext cx="2756408" cy="6299200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>200152</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Connecteur droit avec flèche 47"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="10" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5352796" y="2232152"/>
+          <a:ext cx="2756408" cy="4882896"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="33020">
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Connecteur droit avec flèche 50"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5352796" y="3657600"/>
+          <a:ext cx="2756408" cy="3454400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36830">
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399796</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>155956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>679704</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>111252</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Connecteur droit avec flèche 52"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4527296" y="5032756"/>
+          <a:ext cx="2756408" cy="2190496"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="139700">
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="Connecteur droit avec flèche 57"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9334500" y="815848"/>
+          <a:ext cx="2222500" cy="3657600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="59690">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>197104</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="Connecteur droit avec flèche 60"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9334500" y="2229104"/>
+          <a:ext cx="2222500" cy="2241296"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="20320">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Connecteur droit avec flèche 62"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="11" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9334500" y="3660648"/>
+          <a:ext cx="2222500" cy="812800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="26670">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>3048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>197104</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="Connecteur droit avec flèche 65"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9334500" y="4473448"/>
+          <a:ext cx="2222500" cy="600456"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="127000">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>200152</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="71" name="Connecteur droit avec flèche 70"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="14" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8509000" y="4470400"/>
+          <a:ext cx="2222500" cy="2028952"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="106680">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9126,7 +10539,7 @@
   <dimension ref="A1:I10841"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1041542"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -85165,8 +86578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -85235,4 +86648,446 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-0.61257799999999996</v>
+      </c>
+      <c r="D2">
+        <f>-C2</f>
+        <v>0.61257799999999996</v>
+      </c>
+      <c r="E2" s="3">
+        <f>D2*7.544</f>
+        <v>4.6212884319999992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-0.210651</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D25" si="0">-C3</f>
+        <v>0.210651</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E25" si="1">D3*7.544</f>
+        <v>1.5891511439999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-0.28693200000000002</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.28693200000000002</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="1"/>
+        <v>2.1646150080000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-1.04617</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1.04617</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="1"/>
+        <v>7.8923064800000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-0.56591999999999998</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.56591999999999998</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="1"/>
+        <v>4.2693004799999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-0.212113</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.212113</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>1.6001804719999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-0.18895600000000001</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.18895600000000001</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="1"/>
+        <v>1.4254840639999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-0.80635199999999996</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.80635199999999996</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="1"/>
+        <v>6.0831194879999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="E11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2">
+        <v>-7.2378399999999996E-2</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>7.2378399999999996E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.54602264959999991</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-0.350024</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.350024</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>2.6405810559999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-0.384903</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.384903</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>2.9037082319999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-1.4495199999999999</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1.4495199999999999</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>10.935178879999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2">
+        <v>-0.61736599999999997</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.61736599999999997</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="1"/>
+        <v>4.6574091039999992</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="E18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="2">
+        <v>-0.21399899999999999</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0.21399899999999999</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="1"/>
+        <v>1.6144084559999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="E20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="2">
+        <v>-0.282495</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0.282495</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="1"/>
+        <v>2.1311422799999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="E22" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="2">
+        <v>-1.32558</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>1.32558</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="1"/>
+        <v>10.000175519999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="E24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="2">
+        <v>-1.10782</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>1.10782</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3573940800000006</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
+setteur pour le nombre de mesure en fonction de la taille du fichier d'entrainement +accesseur getArgument pour permettre de demander les valeurs à prédire directement dans les arguments du programme -Training() permet de mettre toute la partie d'entrainement du main() dans la même fonction, plus flexible +fonction du calcul des percentage de chaque neurone de sortie +creation de fichier de donnee pour la prediction de chiffre en fonction de la matrice d'entree + calcNumberTrain qui donne le nombre de valeur pour l'entrainement dans le fichier +commentaire de neural.cpp
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="17540" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="17540" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="moy10" sheetId="2" r:id="rId1"/>
@@ -17,9 +17,11 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId3"/>
     <sheet name="Feuil2" sheetId="4" r:id="rId4"/>
     <sheet name="Feuil3" sheetId="5" r:id="rId5"/>
+    <sheet name="Feuil4" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Feuil1!$A$1:$B$8442</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Feuil4!$A$1:$A$102</definedName>
     <definedName name="_xlnm.Criteria" localSheetId="2">Feuil1!$A$6</definedName>
     <definedName name="_xlnm.Extract" localSheetId="2">Feuil1!$I:$I</definedName>
   </definedNames>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9908" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10010" uniqueCount="30">
   <si>
     <t xml:space="preserve">passe nÂ° </t>
   </si>
@@ -4453,11 +4455,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2091515456"/>
-        <c:axId val="2137150448"/>
+        <c:axId val="2072358768"/>
+        <c:axId val="2110215472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2091515456"/>
+        <c:axId val="2072358768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4466,7 +4468,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137150448"/>
+        <c:crossAx val="2110215472"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4474,7 +4476,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2137150448"/>
+        <c:axId val="2110215472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -4486,7 +4488,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091515456"/>
+        <c:crossAx val="2072358768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8777,11 +8779,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2139262272"/>
-        <c:axId val="2142072960"/>
+        <c:axId val="2111058320"/>
+        <c:axId val="2111061168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2139262272"/>
+        <c:axId val="2111058320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8790,7 +8792,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142072960"/>
+        <c:crossAx val="2111061168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8798,7 +8800,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142072960"/>
+        <c:axId val="2111061168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -8810,7 +8812,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139262272"/>
+        <c:crossAx val="2111058320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8820,6 +8822,939 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="movingAvg"/>
+            <c:period val="10"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil4!$G$1:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.018</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.022</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.056</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.044</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.036</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.057</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.023</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.066</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.015</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.072</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.009</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.076</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.0047</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.0015</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.082</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.0008</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.084</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.0026</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.085</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.0039</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.086</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.0049</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.099</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.087</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.0057</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.099</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.087</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.0063</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.098</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.088</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.0068</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.098</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.088</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.0071</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.097</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2146906032"/>
+        <c:axId val="-2131816448"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2146906032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2131816448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2131816448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2146906032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10273,6 +11208,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -86654,8 +87624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -87090,4 +88060,1149 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>0.1</v>
+      </c>
+      <c r="F1">
+        <v>0.1</v>
+      </c>
+      <c r="G1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="F2">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="G2">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0.16</v>
+      </c>
+      <c r="F3">
+        <v>2.3E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2.3E-2</v>
+      </c>
+      <c r="F4">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0.23</v>
+      </c>
+      <c r="F5">
+        <v>0.04</v>
+      </c>
+      <c r="G5">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="F6">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F7">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="G7">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.04</v>
+      </c>
+      <c r="F8">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G8">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>0.09</v>
+      </c>
+      <c r="F9">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G9">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F10">
+        <v>6.3E-2</v>
+      </c>
+      <c r="G10">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>0.18</v>
+      </c>
+      <c r="F11">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G11">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="F12">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="G12">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F13">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G13">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F14">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="G14">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="F15">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G15">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F16">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G16">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>0.15</v>
+      </c>
+      <c r="F17">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G17">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>6.3E-2</v>
+      </c>
+      <c r="F18">
+        <v>6.2E-2</v>
+      </c>
+      <c r="G18">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F19">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G19">
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="F20">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G20">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F21">
+        <v>6.2E-2</v>
+      </c>
+      <c r="G21">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F22">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G22">
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>0.13</v>
+      </c>
+      <c r="F23">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="G23">
+        <v>4.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F24">
+        <v>6.2E-2</v>
+      </c>
+      <c r="G24">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="F25">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G25">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="F26">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G26">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>2.3E-2</v>
+      </c>
+      <c r="F27">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G27">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="F28">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="G28">
+        <v>8.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>0.12</v>
+      </c>
+      <c r="F29">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G29">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F30">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G30">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F31">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="G31">
+        <v>8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F32">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G32">
+        <v>2.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F33">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G33">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <v>6.2E-2</v>
+      </c>
+      <c r="F34">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G34">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>0.12</v>
+      </c>
+      <c r="F35">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G35">
+        <v>3.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F36">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G36">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F37">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G37">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F38">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G38">
+        <v>4.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F39">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G39">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40">
+        <v>6.2E-2</v>
+      </c>
+      <c r="F40">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G40">
+        <v>8.6999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>0.11</v>
+      </c>
+      <c r="F41">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G41">
+        <v>5.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F42">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G42">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="F43">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G43">
+        <v>8.6999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="F44">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G44">
+        <v>6.3E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="F45">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G45">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>6.2E-2</v>
+      </c>
+      <c r="F46">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G46">
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>0.11</v>
+      </c>
+      <c r="F47">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G47">
+        <v>6.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F48">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G48">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>0.08</v>
+      </c>
+      <c r="F49">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G49">
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F50">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G50">
+        <v>7.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>1.5E-3</v>
+      </c>
+      <c r="F51">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G51">
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="F52">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G52">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <v>8.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56">
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>2.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>3.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75">
+        <v>4.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79">
+        <v>8.6999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81">
+        <v>5.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85">
+        <v>8.6999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87">
+        <v>6.3E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91">
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93">
+        <v>6.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97">
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>6</v>
+      </c>
+      <c r="B98">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99">
+        <v>7.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101">
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:A102"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>